<commit_message>
modified:   deployment_manifests/assets_groups_manifest.csv 	modified:   "\320\270\321\201\321\205\320\276\320\264\320\275\321\213\320\265 \320\274\320\260\320\275\320\270\321\204\320\265\321\201\321\202\321\213/assets_groups_manifest.xlsx"
</commit_message>
<xml_diff>
--- a/исходные манифесты/assets_groups_manifest.xlsx
+++ b/исходные манифесты/assets_groups_manifest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20408"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20409"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\k.krasnovskiy\Work Folders\Desktop\development\git\PT-MP-VM-APi-Python\PT-MP-VM-Api\исходные манифесты\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{392AB74D-1E44-4E39-A811-3ADEE25BCFBF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C7446C1-8983-4DE4-8820-F241E3277EC2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1890" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1890" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="77">
   <si>
     <t>address</t>
   </si>
@@ -69,72 +69,27 @@
     <t>Root</t>
   </si>
   <si>
-    <t>Инфраструктура_2</t>
-  </si>
-  <si>
     <t>Все активы организации</t>
   </si>
   <si>
-    <t>Unix активы_2</t>
-  </si>
-  <si>
     <t>Unix подобные операционные системы</t>
   </si>
   <si>
-    <t>Astra_2</t>
-  </si>
-  <si>
     <t>Хосты под управлением астра линукс</t>
   </si>
   <si>
-    <t>Debian_2</t>
-  </si>
-  <si>
     <t>Хосты под управлением дебиан</t>
   </si>
   <si>
-    <t>Ubuntu_2</t>
-  </si>
-  <si>
-    <t>Хосты под управлением Ubuntu</t>
-  </si>
-  <si>
-    <t>Windows активы_2</t>
-  </si>
-  <si>
     <t>Все Windows активы организации</t>
   </si>
   <si>
-    <t>Windows АРМы_2</t>
-  </si>
-  <si>
-    <t>Рабочие станции пользователей</t>
-  </si>
-  <si>
-    <t>Windows Сервера_2</t>
-  </si>
-  <si>
-    <t>Сервера под управлением Windows ОС</t>
-  </si>
-  <si>
-    <t>Сервисы_2</t>
-  </si>
-  <si>
     <t>Инфраструктурные сервисы организации</t>
   </si>
   <si>
-    <t>DNS-сервера_2</t>
-  </si>
-  <si>
     <t>DNSы</t>
   </si>
   <si>
-    <t>Контроллеры домена_2</t>
-  </si>
-  <si>
-    <t>DC</t>
-  </si>
-  <si>
     <t>Хосты, на которых есть средства управления базами данных</t>
   </si>
   <si>
@@ -192,7 +147,115 @@
     <t>Host.HostRoles.Role = 'DNS Server'</t>
   </si>
   <si>
-    <t>СУБД_2</t>
+    <t>Сети организации</t>
+  </si>
+  <si>
+    <t>Все сети, используемые в организации</t>
+  </si>
+  <si>
+    <t>10.2.118.0/24</t>
+  </si>
+  <si>
+    <t>10.2.139.0/24</t>
+  </si>
+  <si>
+    <t>10.2.183.0/24</t>
+  </si>
+  <si>
+    <t>10.2.55.0/24</t>
+  </si>
+  <si>
+    <t>Инфраструктура</t>
+  </si>
+  <si>
+    <t>Unix активы</t>
+  </si>
+  <si>
+    <t>Astra OS</t>
+  </si>
+  <si>
+    <t>Debian OS</t>
+  </si>
+  <si>
+    <t>Ubuntu OS</t>
+  </si>
+  <si>
+    <t>Хосты под управлением убунту</t>
+  </si>
+  <si>
+    <t>Windows активы</t>
+  </si>
+  <si>
+    <t>Windows АРМы</t>
+  </si>
+  <si>
+    <t>Windows сервера</t>
+  </si>
+  <si>
+    <t>Рабочие станции пользователей под управлением Windows (xp,7,8,10,11)</t>
+  </si>
+  <si>
+    <t>Сервера под управлением Windows (2012, 2016, 2019, 2022)</t>
+  </si>
+  <si>
+    <t>Сервисы</t>
+  </si>
+  <si>
+    <t>Контроллеры домена в организации</t>
+  </si>
+  <si>
+    <t>Сеть, принадлежащая Кириллу У</t>
+  </si>
+  <si>
+    <t>Сеть, принадлежащая Кириллу Б</t>
+  </si>
+  <si>
+    <t>Сеть, принадлежащая Кириллу К</t>
+  </si>
+  <si>
+    <t>Сеть, принадлежащая Виктору Т</t>
+  </si>
+  <si>
+    <t>ОПС</t>
+  </si>
+  <si>
+    <t>ОСМР</t>
+  </si>
+  <si>
+    <t>Сети отдела прикладных систем</t>
+  </si>
+  <si>
+    <t>Сети отдела систем мониторинга и реагирования</t>
+  </si>
+  <si>
+    <t>Host.IpAddress in 10.2.183.0/24</t>
+  </si>
+  <si>
+    <t>Host.IpAddress in 10.2.55.0/24</t>
+  </si>
+  <si>
+    <t>Host.IpAddress in 10.2.139.0/24</t>
+  </si>
+  <si>
+    <t>Host.IpAddress in 10.2.118.0/24</t>
+  </si>
+  <si>
+    <t>DNS-сервера</t>
+  </si>
+  <si>
+    <t>Контроллеры домена</t>
+  </si>
+  <si>
+    <t>СУБД</t>
+  </si>
+  <si>
+    <t>WEB-сервера</t>
+  </si>
+  <si>
+    <t>Хосты, на которых развернуты веб-сервисы</t>
+  </si>
+  <si>
+    <t>Host.HostRoles.Role = 'Web Server'</t>
   </si>
 </sst>
 </file>
@@ -510,57 +573,57 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q13"/>
+  <dimension ref="A1:Q21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.1796875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.7265625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="22.453125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.140625" customWidth="1"/>
+    <col min="3" max="3" width="22.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="B1" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="C1" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="D1" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="E1" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="F1" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="G1" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="H1" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="I1" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="J1" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="K1" t="s">
         <v>0</v>
@@ -584,12 +647,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" t="s">
         <v>14</v>
-      </c>
-      <c r="B2" t="s">
-        <v>15</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
@@ -613,15 +676,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>47</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>46</v>
       </c>
       <c r="D3" t="s">
         <v>12</v>
@@ -642,21 +705,21 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>48</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>47</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="F4" t="s">
         <v>8</v>
@@ -674,21 +737,21 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>49</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>47</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="F5" t="s">
         <v>10</v>
@@ -706,21 +769,21 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>47</v>
       </c>
       <c r="D6" t="s">
         <v>7</v>
       </c>
       <c r="E6" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="F6" t="s">
         <v>9</v>
@@ -738,21 +801,21 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>52</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>46</v>
       </c>
       <c r="D7" t="s">
         <v>12</v>
       </c>
       <c r="F7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G7" t="s">
         <v>9</v>
@@ -761,27 +824,27 @@
         <v>11</v>
       </c>
       <c r="I7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="J7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>53</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>55</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
+        <v>52</v>
       </c>
       <c r="D8" t="s">
         <v>7</v>
       </c>
       <c r="E8" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="F8" t="s">
         <v>11</v>
@@ -790,7 +853,7 @@
         <v>9</v>
       </c>
       <c r="H8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I8" t="s">
         <v>11</v>
@@ -799,24 +862,24 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>56</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
+        <v>52</v>
       </c>
       <c r="D9" t="s">
         <v>7</v>
       </c>
       <c r="E9" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="F9" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G9" t="s">
         <v>9</v>
@@ -825,21 +888,21 @@
         <v>11</v>
       </c>
       <c r="I9" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="J9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>57</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>14</v>
+        <v>46</v>
       </c>
       <c r="D10" t="s">
         <v>12</v>
@@ -860,21 +923,21 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>32</v>
+        <v>71</v>
       </c>
       <c r="B11" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
+        <v>57</v>
       </c>
       <c r="D11" t="s">
         <v>7</v>
       </c>
       <c r="E11" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="F11" t="s">
         <v>10</v>
@@ -892,21 +955,21 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>72</v>
       </c>
       <c r="B12" t="s">
-        <v>35</v>
+        <v>58</v>
       </c>
       <c r="C12" t="s">
-        <v>30</v>
+        <v>57</v>
       </c>
       <c r="D12" t="s">
         <v>7</v>
       </c>
       <c r="E12" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="F12" t="s">
         <v>8</v>
@@ -924,21 +987,21 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>55</v>
+        <v>73</v>
       </c>
       <c r="B13" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="C13" t="s">
-        <v>30</v>
+        <v>57</v>
       </c>
       <c r="D13" t="s">
         <v>7</v>
       </c>
       <c r="E13" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="F13" t="s">
         <v>10</v>
@@ -953,6 +1016,223 @@
         <v>10</v>
       </c>
       <c r="J13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>74</v>
+      </c>
+      <c r="B14" t="s">
+        <v>75</v>
+      </c>
+      <c r="C14" t="s">
+        <v>57</v>
+      </c>
+      <c r="D14" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" t="s">
+        <v>76</v>
+      </c>
+      <c r="F14" t="s">
+        <v>8</v>
+      </c>
+      <c r="G14" t="s">
+        <v>9</v>
+      </c>
+      <c r="H14" t="s">
+        <v>11</v>
+      </c>
+      <c r="I14" t="s">
+        <v>10</v>
+      </c>
+      <c r="J14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" t="s">
+        <v>9</v>
+      </c>
+      <c r="G15" t="s">
+        <v>9</v>
+      </c>
+      <c r="H15" t="s">
+        <v>9</v>
+      </c>
+      <c r="I15" t="s">
+        <v>9</v>
+      </c>
+      <c r="J15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16" t="s">
+        <v>65</v>
+      </c>
+      <c r="C16" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>64</v>
+      </c>
+      <c r="B17" t="s">
+        <v>66</v>
+      </c>
+      <c r="C17" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" t="s">
+        <v>64</v>
+      </c>
+      <c r="D18" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" t="s">
+        <v>70</v>
+      </c>
+      <c r="F18" t="s">
+        <v>11</v>
+      </c>
+      <c r="G18" t="s">
+        <v>9</v>
+      </c>
+      <c r="H18" t="s">
+        <v>10</v>
+      </c>
+      <c r="I18" t="s">
+        <v>10</v>
+      </c>
+      <c r="J18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" t="s">
+        <v>60</v>
+      </c>
+      <c r="C19" t="s">
+        <v>63</v>
+      </c>
+      <c r="D19" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" t="s">
+        <v>69</v>
+      </c>
+      <c r="F19" t="s">
+        <v>10</v>
+      </c>
+      <c r="G19" t="s">
+        <v>9</v>
+      </c>
+      <c r="H19" t="s">
+        <v>11</v>
+      </c>
+      <c r="I19" t="s">
+        <v>8</v>
+      </c>
+      <c r="J19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20" t="s">
+        <v>63</v>
+      </c>
+      <c r="D20" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" t="s">
+        <v>67</v>
+      </c>
+      <c r="F20" t="s">
+        <v>8</v>
+      </c>
+      <c r="G20" t="s">
+        <v>9</v>
+      </c>
+      <c r="H20" t="s">
+        <v>10</v>
+      </c>
+      <c r="I20" t="s">
+        <v>8</v>
+      </c>
+      <c r="J20" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" t="s">
+        <v>62</v>
+      </c>
+      <c r="C21" t="s">
+        <v>63</v>
+      </c>
+      <c r="D21" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" t="s">
+        <v>68</v>
+      </c>
+      <c r="F21" t="s">
+        <v>8</v>
+      </c>
+      <c r="G21" t="s">
+        <v>9</v>
+      </c>
+      <c r="H21" t="s">
+        <v>8</v>
+      </c>
+      <c r="I21" t="s">
+        <v>8</v>
+      </c>
+      <c r="J21" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>